<commit_message>
BE + FE Fix Actors Working Hour Report query check (date format) + Add Client info in XLS
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/CRA _COMPANY_ _DATE_.xlsx
+++ b/Ressources/DocTemplates/CRA _COMPANY_ _DATE_.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFBFE0A-757C-4491-A560-8A7548306C75}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98389026-DE9A-4DE6-93D7-571C33AFFC61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="7965" windowWidth="24540" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="4740" windowWidth="42870" windowHeight="25830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRA" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CRA!$B$4:$L$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CRA!$B$4:$M$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">CRA!$1:$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">CRA!$B:$J</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Jour de Début</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Société</t>
+  </si>
+  <si>
+    <t>Client</t>
   </si>
 </sst>
 </file>
@@ -792,10 +795,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L944"/>
+  <dimension ref="A1:M944"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -809,7 +812,7 @@
     <col min="11" max="11" width="8.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -825,8 +828,8 @@
       <c r="I1" s="10"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="32" t="s">
         <v>8</v>
       </c>
@@ -849,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
@@ -872,8 +875,11 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="18"/>
       <c r="D5" s="19"/>
@@ -884,7 +890,7 @@
       <c r="I5" s="21"/>
       <c r="J5" s="22"/>
     </row>
-    <row r="6" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="24"/>
       <c r="C6" s="25"/>
@@ -896,7 +902,7 @@
       <c r="I6" s="28"/>
       <c r="J6" s="29"/>
     </row>
-    <row r="7" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="24"/>
       <c r="C7" s="25"/>
       <c r="D7" s="26"/>
@@ -907,7 +913,7 @@
       <c r="I7" s="28"/>
       <c r="J7" s="29"/>
     </row>
-    <row r="8" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
       <c r="D8" s="26"/>
@@ -918,7 +924,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="29"/>
     </row>
-    <row r="9" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
@@ -929,7 +935,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="29"/>
     </row>
-    <row r="10" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="24"/>
       <c r="C10" s="25"/>
       <c r="D10" s="26"/>
@@ -940,7 +946,7 @@
       <c r="I10" s="28"/>
       <c r="J10" s="29"/>
     </row>
-    <row r="11" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
       <c r="D11" s="26"/>
@@ -951,7 +957,7 @@
       <c r="I11" s="28"/>
       <c r="J11" s="29"/>
     </row>
-    <row r="12" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="24"/>
       <c r="C12" s="25"/>
       <c r="D12" s="26"/>
@@ -962,7 +968,7 @@
       <c r="I12" s="28"/>
       <c r="J12" s="29"/>
     </row>
-    <row r="13" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="24"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
@@ -973,7 +979,7 @@
       <c r="I13" s="28"/>
       <c r="J13" s="29"/>
     </row>
-    <row r="14" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="26"/>
@@ -984,7 +990,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
     </row>
-    <row r="15" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
       <c r="D15" s="26"/>
@@ -995,7 +1001,7 @@
       <c r="I15" s="28"/>
       <c r="J15" s="29"/>
     </row>
-    <row r="16" spans="1:12" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
       <c r="D16" s="26"/>
@@ -11215,7 +11221,7 @@
       <c r="J944" s="29"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:L4" xr:uid="{A1444CA0-D29A-4386-B63C-D77A657D83D0}"/>
+  <autoFilter ref="B4:M4" xr:uid="{9FF99E08-F36C-4CEE-BAC8-3791673D62DA}"/>
   <mergeCells count="6">
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>